<commit_message>
RDM-4525 Merge missing AuthorisationComplexType tab from RDM-4084
</commit_message>
<xml_diff>
--- a/application/src/test/resources/CCD_TestDefinition_V45_RDM-4525.xlsx
+++ b/application/src/test/resources/CCD_TestDefinition_V45_RDM-4525.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="-14060" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="500" firstSheet="1" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Jurisdiction" sheetId="1" r:id="rId1"/>
@@ -29,12 +29,13 @@
     <sheet name="CaseRoles" sheetId="20" r:id="rId15"/>
     <sheet name="AuthorisationCaseType" sheetId="15" r:id="rId16"/>
     <sheet name="AuthorisationCaseField" sheetId="16" r:id="rId17"/>
-    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId18"/>
-    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId19"/>
-    <sheet name="SearchAlias" sheetId="22" r:id="rId20"/>
+    <sheet name="AuthorisationComplexType" sheetId="23" r:id="rId18"/>
+    <sheet name="AuthorisationCaseEvent" sheetId="17" r:id="rId19"/>
+    <sheet name="AuthorisationCaseState" sheetId="18" r:id="rId20"/>
+    <sheet name="SearchAlias" sheetId="22" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CaseField!$A$1:$M$32</definedName>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="338">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1327" uniqueCount="344">
   <si>
     <t>Jurisdiction</t>
   </si>
@@ -1081,6 +1082,29 @@
   </si>
   <si>
     <t>Dynamic List</t>
+  </si>
+  <si>
+    <t>AuthorisationComplexType</t>
+  </si>
+  <si>
+    <t>Must match ID on 'CaseType' tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The Field ID should match an ID in the CaseField Tab
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>The complex type element (field) ID (ListElementId) should match the field attribute name used by the service team in creating the case
+MaxLength: 70</t>
+  </si>
+  <si>
+    <t>Must match ID role.  If a role doesn’t have a Row below that mean no access to.
+MaxLength: 100.</t>
+  </si>
+  <si>
+    <t>C - Create, R - Read, U - Update, D - Delete
+MustBe1OrManyOf: &lt;C,R,U,D&gt; MaxLength: 5</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1643,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1628,8 +1652,10 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1877,8 +1903,25 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="8" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="0" xfId="8" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="8" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="9"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -1887,6 +1930,8 @@
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="7"/>
+    <cellStyle name="Normal 2 3" xfId="8"/>
+    <cellStyle name="Normal 3" xfId="9"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8023,6 +8068,185 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="A1" s="185" t="s">
+        <v>338</v>
+      </c>
+      <c r="B1" s="186" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="187" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="188" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="189"/>
+      <c r="F1" s="189"/>
+      <c r="G1" s="189"/>
+    </row>
+    <row r="2" spans="1:7" ht="182" x14ac:dyDescent="0.15">
+      <c r="A2" s="190"/>
+      <c r="B2" s="190"/>
+      <c r="C2" s="191" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="191" t="s">
+        <v>340</v>
+      </c>
+      <c r="E2" s="191" t="s">
+        <v>341</v>
+      </c>
+      <c r="F2" s="191" t="s">
+        <v>342</v>
+      </c>
+      <c r="G2" s="191" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="192" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="192" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="193" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="193" t="s">
+        <v>193</v>
+      </c>
+      <c r="E3" s="193" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="192" t="s">
+        <v>247</v>
+      </c>
+      <c r="G3" s="192" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A4" s="194">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="189"/>
+      <c r="C4" s="195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="196" t="s">
+        <v>54</v>
+      </c>
+      <c r="E4" s="196" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" s="197" t="s">
+        <v>249</v>
+      </c>
+      <c r="G4" s="189" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A5" s="194">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="189"/>
+      <c r="C5" s="195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="196" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="196" t="s">
+        <v>121</v>
+      </c>
+      <c r="F5" s="197" t="s">
+        <v>249</v>
+      </c>
+      <c r="G5" s="189" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="194">
+        <v>42736</v>
+      </c>
+      <c r="B6" s="189"/>
+      <c r="C6" s="195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="196" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="196" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="197" t="s">
+        <v>249</v>
+      </c>
+      <c r="G6" s="189" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="194">
+        <v>42736</v>
+      </c>
+      <c r="B7" s="189"/>
+      <c r="C7" s="195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="196" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="196" t="s">
+        <v>125</v>
+      </c>
+      <c r="F7" s="197" t="s">
+        <v>249</v>
+      </c>
+      <c r="G7" s="189" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A8" s="194">
+        <v>42736</v>
+      </c>
+      <c r="B8" s="189"/>
+      <c r="C8" s="195" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="196" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="196" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" s="197" t="s">
+        <v>249</v>
+      </c>
+      <c r="G8" s="189" t="s">
+        <v>250</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
@@ -12049,7 +12273,375 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="31.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11" style="1" customWidth="1"/>
+    <col min="10" max="14" width="8.83203125" style="1" customWidth="1"/>
+    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+    </row>
+    <row r="2" spans="1:14" ht="74" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+    </row>
+    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="9">
+        <v>42736</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="9">
+        <v>42736</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+    </row>
+    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="9"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="9"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="21"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="21"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+    </row>
+    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="21"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="21"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+    </row>
+    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="21"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="21"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IU15"/>
   <sheetViews>
@@ -12933,375 +13525,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N17"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="14.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="15.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.83203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" customWidth="1"/>
-    <col min="10" max="14" width="8.83203125" style="1" customWidth="1"/>
-    <col min="15" max="1025" width="8.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-    </row>
-    <row r="2" spans="1:14" ht="74" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="9">
-        <v>42736</v>
-      </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="9">
-        <v>42736</v>
-      </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-    </row>
-    <row r="6" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="9"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-    </row>
-    <row r="7" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="9"/>
-      <c r="B7" s="16"/>
-      <c r="C7" s="19"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-    </row>
-    <row r="8" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-    </row>
-    <row r="10" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-    </row>
-    <row r="11" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="21"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="21"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-    </row>
-    <row r="13" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="21"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-    </row>
-    <row r="14" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="21"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
-    </row>
-    <row r="15" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="21"/>
-      <c r="B15" s="9"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="21"/>
-      <c r="B16" s="9"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-      <c r="M17" s="4"/>
-      <c r="N17" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.3"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -14929,7 +15153,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>

</xml_diff>